<commit_message>
neue classes wurde eingefugt
</commit_message>
<xml_diff>
--- a/com.Batch44POM/src/test/java/resources/ulkeler.xlsx
+++ b/com.Batch44POM/src/test/java/resources/ulkeler.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CB33B-669E-47A2-95A0-4D1E55E9CD82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D1A50-D932-4B32-9800-BBC0BE1CCF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="577">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1741,6 +1741,41 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>ilk sutun key, digerleri value olsun</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>"Belarus"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1A1A1A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve"> "Minsk, Belarus, Minsk"</t>
+    </r>
   </si>
   <si>
     <t>NUFUS</t>
@@ -1754,7 +1789,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1773,6 +1808,20 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
@@ -1804,7 +1853,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1864,11 +1913,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1892,6 +1950,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2174,18 +2235,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.28515625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2199,10 +2261,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2230,10 +2292,13 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>576</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2247,7 +2312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2261,7 +2326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2275,7 +2340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2303,7 +2368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -2317,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2331,7 +2396,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -2345,7 +2410,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -2359,7 +2424,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -2373,7 +2438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -2387,7 +2452,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -2401,7 +2466,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -2415,7 +2480,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2428,8 +2493,11 @@
       <c r="D17" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -2443,7 +2511,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -2457,7 +2525,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -2471,7 +2539,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -2485,7 +2553,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -2499,7 +2567,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>68</v>
       </c>
@@ -2513,7 +2581,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>72</v>
       </c>
@@ -2527,7 +2595,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -2541,7 +2609,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>78</v>
       </c>
@@ -2555,7 +2623,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>80</v>
       </c>
@@ -2569,7 +2637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -2583,7 +2651,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>86</v>
       </c>
@@ -2597,7 +2665,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>88</v>
       </c>
@@ -2611,7 +2679,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
@@ -2625,7 +2693,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>94</v>
       </c>
@@ -4873,14 +4941,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>